<commit_message>
added site metadata and river shapefiles
</commit_message>
<xml_diff>
--- a/data/prepped/site_metadata/rt_site_metadata.xlsx
+++ b/data/prepped/site_metadata/rt_site_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikea\Desktop\rt_temp\fixed_site_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\site_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1A6759-FE65-48CC-A974-ED58AE2DFF81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842606D1-38FC-4917-994E-621C3652CA3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33615" yWindow="3090" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_metadata" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -663,10 +663,10 @@
         <v>31</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
finished draft RT site metadata and added PTAGIS site metadata
</commit_message>
<xml_diff>
--- a/data/prepped/site_metadata/rt_site_metadata.xlsx
+++ b/data/prepped/site_metadata/rt_site_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\site_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842606D1-38FC-4917-994E-621C3652CA3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90776B3B-AE50-4C84-A028-B748795101EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33615" yWindow="3090" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="125">
   <si>
     <t>site_name</t>
   </si>
@@ -120,27 +120,12 @@
     <t>site_type</t>
   </si>
   <si>
-    <t>contact_agency</t>
-  </si>
-  <si>
     <t>point_x</t>
   </si>
   <si>
     <t>point_y</t>
   </si>
   <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>BLM</t>
-  </si>
-  <si>
-    <t>IDFG</t>
-  </si>
-  <si>
-    <t>Nez Perce Clearwater NF</t>
-  </si>
-  <si>
     <t>use17_18</t>
   </si>
   <si>
@@ -174,9 +159,6 @@
     <t>YP</t>
   </si>
   <si>
-    <t>Salmon Challis NF</t>
-  </si>
-  <si>
     <t>Upper Lemhi RST</t>
   </si>
   <si>
@@ -204,12 +186,6 @@
     <t>rt_site_type</t>
   </si>
   <si>
-    <t>release</t>
-  </si>
-  <si>
-    <t>observation</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -273,7 +249,157 @@
     <t>trailer</t>
   </si>
   <si>
-    <t>rkm</t>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>rt_fixed</t>
+  </si>
+  <si>
+    <t>rt_roving</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>RV</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>EVL</t>
+  </si>
+  <si>
+    <t>S3A</t>
+  </si>
+  <si>
+    <t>S3B</t>
+  </si>
+  <si>
+    <t>BHC</t>
+  </si>
+  <si>
+    <t>S2O</t>
+  </si>
+  <si>
+    <t>S2I</t>
+  </si>
+  <si>
+    <t>EVU</t>
+  </si>
+  <si>
+    <t>WPC</t>
+  </si>
+  <si>
+    <t>KEN</t>
+  </si>
+  <si>
+    <t>AGC</t>
+  </si>
+  <si>
+    <t>LRW</t>
+  </si>
+  <si>
+    <t>HYC</t>
+  </si>
+  <si>
+    <t>pit_array</t>
+  </si>
+  <si>
+    <t>Lower Lemhi River</t>
+  </si>
+  <si>
+    <t>ptagis_rkm</t>
+  </si>
+  <si>
+    <t>rt_rkm</t>
+  </si>
+  <si>
+    <t>522.303.416.001</t>
+  </si>
+  <si>
+    <t>Eagle Valley Ranch - Lower</t>
+  </si>
+  <si>
+    <t>Eagle Valley Ranch - Upper</t>
+  </si>
+  <si>
+    <t>522.303.416.016</t>
+  </si>
+  <si>
+    <t>522.303.416.020</t>
+  </si>
+  <si>
+    <t>Eagle Valley Ranch S3A</t>
+  </si>
+  <si>
+    <t>Eagle Valley Ranch S3B</t>
+  </si>
+  <si>
+    <t>522.303.416.017</t>
+  </si>
+  <si>
+    <t>Bohannon Creek Lemhi R Basin</t>
+  </si>
+  <si>
+    <t>522.303.416.017.001</t>
+  </si>
+  <si>
+    <t>Lemhi Sub-reach 2 SC Outlet</t>
+  </si>
+  <si>
+    <t>Lemhi Sub-reach 2 SC Inlet</t>
+  </si>
+  <si>
+    <t>522.303.416.018</t>
+  </si>
+  <si>
+    <t>Wimpey Creek, Lemhi R. Basin</t>
+  </si>
+  <si>
+    <t>522.303.416.020.001</t>
+  </si>
+  <si>
+    <t>Kenney Creek In-stream Arrays</t>
+  </si>
+  <si>
+    <t>522.303.416.029.000</t>
+  </si>
+  <si>
+    <t>Agency Creek, Lemhi R. Basin</t>
+  </si>
+  <si>
+    <t>522.303.416.039.001</t>
+  </si>
+  <si>
+    <t>Lemhi River Weir</t>
+  </si>
+  <si>
+    <t>522.303.416.050</t>
+  </si>
+  <si>
+    <t>Hayden Creek In-stream Array</t>
+  </si>
+  <si>
+    <t>522.303.416.049.001</t>
+  </si>
+  <si>
+    <t>522.303.416.049</t>
+  </si>
+  <si>
+    <t>522.303.416.007</t>
+  </si>
+  <si>
+    <t>522.303.489.002</t>
+  </si>
+  <si>
+    <t>roving</t>
+  </si>
+  <si>
+    <t>Roving Receiver 17_18</t>
+  </si>
+  <si>
+    <t>Roving Receiver 19_20</t>
   </si>
 </sst>
 </file>
@@ -626,24 +752,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="5"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -657,508 +784,508 @@
         <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44.869202999999999</v>
       </c>
       <c r="F2" s="2">
-        <v>44.869202999999999</v>
-      </c>
-      <c r="G2" s="2">
         <v>-113.625139</v>
       </c>
+      <c r="G2" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44.861395000000002</v>
       </c>
       <c r="F3" s="2">
-        <v>44.861395000000002</v>
-      </c>
-      <c r="G3" s="2">
         <v>-113.632059</v>
       </c>
+      <c r="G3" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="E4" s="7">
+        <v>45.159500000000001</v>
       </c>
       <c r="F4" s="7">
-        <v>45.159500000000001</v>
-      </c>
-      <c r="G4" s="7">
         <v>-113.8331</v>
       </c>
+      <c r="G4" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="5" t="b">
-        <v>1</v>
+      <c r="J4" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>53</v>
+      </c>
+      <c r="E5" s="7">
+        <v>44.684525999999998</v>
       </c>
       <c r="F5" s="7">
-        <v>44.684525999999998</v>
-      </c>
-      <c r="G5" s="7">
         <v>-114.04047300000001</v>
       </c>
+      <c r="G5" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H5" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44.882640000000002</v>
       </c>
       <c r="F6" s="2">
-        <v>44.882640000000002</v>
-      </c>
-      <c r="G6" s="2">
         <v>-113.62936000000001</v>
       </c>
+      <c r="G6" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H6" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>34</v>
+      <c r="E7" s="2">
+        <v>44.9831</v>
       </c>
       <c r="F7" s="2">
-        <v>44.9831</v>
-      </c>
-      <c r="G7" s="2">
         <v>-113.64709499999999</v>
       </c>
+      <c r="G7" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E8" s="7">
+        <v>45.016910000000003</v>
       </c>
       <c r="F8" s="7">
-        <v>45.016910000000003</v>
-      </c>
-      <c r="G8" s="7">
         <v>-113.65719</v>
       </c>
+      <c r="G8" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E9" s="7">
+        <v>45.042450000000002</v>
       </c>
       <c r="F9" s="7">
-        <v>45.042450000000002</v>
-      </c>
-      <c r="G9" s="7">
         <v>-113.6767</v>
       </c>
+      <c r="G9" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E10" s="7">
+        <v>45.100087000000002</v>
       </c>
       <c r="F10" s="7">
-        <v>45.100087000000002</v>
-      </c>
-      <c r="G10" s="7">
         <v>-113.72604200000001</v>
       </c>
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H10" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E11" s="7">
+        <v>45.115009999999998</v>
       </c>
       <c r="F11" s="7">
-        <v>45.115009999999998</v>
-      </c>
-      <c r="G11" s="7">
         <v>-113.77392</v>
       </c>
+      <c r="G11" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H11" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E12" s="7">
+        <v>45.115009999999998</v>
       </c>
       <c r="F12" s="7">
-        <v>45.115009999999998</v>
-      </c>
-      <c r="G12" s="7">
         <v>-113.77392</v>
       </c>
+      <c r="G12" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H12" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E13" s="7">
+        <v>45.157769999999999</v>
       </c>
       <c r="F13" s="7">
-        <v>45.157769999999999</v>
-      </c>
-      <c r="G13" s="7">
         <v>-113.82239</v>
       </c>
+      <c r="G13" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="E14" s="7">
+        <v>45.160139999999998</v>
       </c>
       <c r="F14" s="7">
-        <v>45.160139999999998</v>
-      </c>
-      <c r="G14" s="7">
         <v>-113.83905</v>
       </c>
+      <c r="G14" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H14" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>36</v>
+        <v>72</v>
+      </c>
+      <c r="E15" s="8">
+        <v>44.700719999999997</v>
       </c>
       <c r="F15" s="8">
-        <v>44.700719999999997</v>
-      </c>
-      <c r="G15" s="8">
         <v>-114.04404</v>
       </c>
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>35</v>
+        <v>72</v>
+      </c>
+      <c r="E16" s="8">
+        <v>44.909619999999997</v>
       </c>
       <c r="F16" s="8">
-        <v>44.909619999999997</v>
-      </c>
-      <c r="G16" s="8">
         <v>-113.96426</v>
       </c>
+      <c r="G16" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1169,28 +1296,28 @@
         <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E17" s="8">
+        <v>45.1710059778</v>
       </c>
       <c r="F17" s="8">
-        <v>45.1710059778</v>
-      </c>
-      <c r="G17" s="8">
         <v>-113.910351732</v>
       </c>
+      <c r="G17" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I17" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4" t="b">
-        <v>1</v>
+      <c r="I17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1201,60 +1328,60 @@
         <v>12</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E18" s="8">
+        <v>45.186379416900003</v>
       </c>
       <c r="F18" s="8">
-        <v>45.186379416900003</v>
-      </c>
-      <c r="G18" s="8">
         <v>-113.891305307</v>
       </c>
+      <c r="G18" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4" t="b">
-        <v>1</v>
+      <c r="I18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E19" s="7">
+        <v>45.231563999999999</v>
       </c>
       <c r="F19" s="7">
-        <v>45.231563999999999</v>
-      </c>
-      <c r="G19" s="7">
         <v>-113.89469200000001</v>
       </c>
+      <c r="G19" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1265,28 +1392,28 @@
         <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>35</v>
+        <v>72</v>
+      </c>
+      <c r="E20" s="8">
+        <v>45.253070000000001</v>
       </c>
       <c r="F20" s="8">
-        <v>45.253070000000001</v>
-      </c>
-      <c r="G20" s="8">
         <v>-113.90602</v>
       </c>
-      <c r="H20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="4" t="b">
-        <v>1</v>
+      <c r="G20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1297,28 +1424,28 @@
         <v>14</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>35</v>
+        <v>72</v>
+      </c>
+      <c r="E21" s="8">
+        <v>45.3109427049</v>
       </c>
       <c r="F21" s="8">
-        <v>45.3109427049</v>
-      </c>
-      <c r="G21" s="8">
         <v>-113.906460821</v>
       </c>
+      <c r="G21" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="4" t="b">
-        <v>1</v>
+      <c r="I21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1329,28 +1456,28 @@
         <v>15</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
+      </c>
+      <c r="E22" s="8">
+        <v>45.346179999999997</v>
       </c>
       <c r="F22" s="8">
-        <v>45.346179999999997</v>
-      </c>
-      <c r="G22" s="8">
         <v>-113.92242</v>
       </c>
+      <c r="G22" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H22" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" s="4" t="b">
-        <v>0</v>
+      <c r="I22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1361,28 +1488,28 @@
         <v>16</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
+      </c>
+      <c r="E23" s="8">
+        <v>45.360959999999999</v>
       </c>
       <c r="F23" s="8">
-        <v>45.360959999999999</v>
-      </c>
-      <c r="G23" s="8">
         <v>-113.96332</v>
       </c>
-      <c r="H23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4" t="b">
-        <v>0</v>
+      <c r="G23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1393,28 +1520,28 @@
         <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="E24" s="8">
+        <v>45.395519999999998</v>
       </c>
       <c r="F24" s="8">
-        <v>45.395519999999998</v>
-      </c>
-      <c r="G24" s="8">
         <v>-113.97883</v>
       </c>
+      <c r="G24" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H24" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I24" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="4" t="b">
-        <v>1</v>
+      <c r="I24" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1425,28 +1552,28 @@
         <v>18</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>49</v>
+        <v>72</v>
+      </c>
+      <c r="E25" s="8">
+        <v>45.379770000000001</v>
       </c>
       <c r="F25" s="8">
-        <v>45.379770000000001</v>
-      </c>
-      <c r="G25" s="8">
         <v>-114.07088</v>
       </c>
+      <c r="G25" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H25" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I25" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="4" t="b">
-        <v>1</v>
+      <c r="I25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1457,28 +1584,28 @@
         <v>19</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="E26" s="8">
+        <v>45.403799999999997</v>
       </c>
       <c r="F26" s="8">
-        <v>45.403799999999997</v>
-      </c>
-      <c r="G26" s="8">
         <v>-114.215816667</v>
       </c>
+      <c r="G26" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I26" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="4" t="b">
-        <v>1</v>
+      <c r="I26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1489,28 +1616,28 @@
         <v>20</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="E27" s="8">
+        <v>45.300644939500003</v>
       </c>
       <c r="F27" s="8">
-        <v>45.300644939500003</v>
-      </c>
-      <c r="G27" s="8">
         <v>-114.53440792400001</v>
       </c>
+      <c r="G27" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H27" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" s="4" t="b">
-        <v>1</v>
+      <c r="I27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1521,60 +1648,60 @@
         <v>21</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="E28" s="8">
+        <v>45.369770000000003</v>
       </c>
       <c r="F28" s="8">
-        <v>45.369770000000003</v>
-      </c>
-      <c r="G28" s="8">
         <v>-114.68715</v>
       </c>
+      <c r="G28" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4" t="b">
-        <v>1</v>
+      <c r="I28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="E29" s="8">
+        <v>45.543717000000001</v>
       </c>
       <c r="F29" s="8">
-        <v>45.543717000000001</v>
-      </c>
-      <c r="G29" s="8">
         <v>-115.249965</v>
       </c>
+      <c r="G29" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="H29" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" s="4" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="I29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1585,28 +1712,28 @@
         <v>22</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>37</v>
+        <v>73</v>
+      </c>
+      <c r="E30" s="8">
+        <v>45.4595545882</v>
       </c>
       <c r="F30" s="8">
-        <v>45.4595545882</v>
-      </c>
-      <c r="G30" s="8">
         <v>-115.89275433100001</v>
       </c>
+      <c r="G30" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H30" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I30" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" s="4" t="b">
-        <v>0</v>
+      <c r="I30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1617,28 +1744,28 @@
         <v>23</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>35</v>
+        <v>72</v>
+      </c>
+      <c r="E31" s="8">
+        <v>45.413427686600002</v>
       </c>
       <c r="F31" s="8">
-        <v>45.413427686600002</v>
-      </c>
-      <c r="G31" s="8">
         <v>-116.302723699</v>
       </c>
+      <c r="G31" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H31" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I31" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" s="4" t="b">
-        <v>0</v>
+      <c r="I31" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1649,29 +1776,518 @@
         <v>24</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="8">
+        <v>45.660486265999999</v>
+      </c>
+      <c r="F32" s="8">
+        <v>-116.29227192800001</v>
+      </c>
+      <c r="G32" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="1">
+        <v>45.176475000000003</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-113.885278</v>
+      </c>
+      <c r="G35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="8">
-        <v>45.660486265999999</v>
-      </c>
-      <c r="G32" s="8">
-        <v>-116.29227192800001</v>
-      </c>
-      <c r="H32" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="C36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="1">
+        <v>45.115074</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-113.774021</v>
+      </c>
+      <c r="G36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="1">
+        <v>45.113169999999997</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-113.7556</v>
+      </c>
+      <c r="G37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="1">
+        <v>45.112769999999998</v>
+      </c>
+      <c r="F38" s="1">
+        <v>-113.74987</v>
+      </c>
+      <c r="G38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="1">
+        <v>45.112189000000001</v>
+      </c>
+      <c r="F39" s="1">
+        <v>-113.746897</v>
+      </c>
+      <c r="G39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="1">
+        <v>45.111257000000002</v>
+      </c>
+      <c r="F40" s="1">
+        <v>-113.74641800000001</v>
+      </c>
+      <c r="G40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="1">
+        <v>45.109456999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-113.742696</v>
+      </c>
+      <c r="G41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="1">
+        <v>45.100087000000002</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-113.72604200000001</v>
+      </c>
+      <c r="G42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="1">
+        <v>45.097937999999999</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-113.72049699999999</v>
+      </c>
+      <c r="G43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="1">
+        <v>45.026792</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-113.654847</v>
+      </c>
+      <c r="G44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="1">
+        <v>44.956738999999999</v>
+      </c>
+      <c r="F45" s="1">
+        <v>-113.639543</v>
+      </c>
+      <c r="G45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="1">
+        <v>44.865960029999997</v>
+      </c>
+      <c r="F46" s="1">
+        <v>-113.62472099999999</v>
+      </c>
+      <c r="G46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="1">
+        <v>44.861654000000001</v>
+      </c>
+      <c r="F47" s="1">
+        <v>-113.63193699999999</v>
+      </c>
+      <c r="G47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D48" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added final river, site, and rkm shapefiles and cleaned up directories
</commit_message>
<xml_diff>
--- a/data/prepped/site_metadata/rt_site_metadata.xlsx
+++ b/data/prepped/site_metadata/rt_site_metadata.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\site_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90776B3B-AE50-4C84-A028-B748795101EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB667974-4979-400F-A58C-7DAB6D51299E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_metadata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="125">
   <si>
     <t>site_name</t>
   </si>
@@ -255,15 +261,6 @@
     <t>rt_fixed</t>
   </si>
   <si>
-    <t>rt_roving</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>RV</t>
-  </si>
-  <si>
     <t>LLR</t>
   </si>
   <si>
@@ -393,13 +390,22 @@
     <t>522.303.489.002</t>
   </si>
   <si>
-    <t>roving</t>
-  </si>
-  <si>
-    <t>Roving Receiver 17_18</t>
-  </si>
-  <si>
-    <t>Roving Receiver 19_20</t>
+    <t>USE</t>
+  </si>
+  <si>
+    <t>USI</t>
+  </si>
+  <si>
+    <t>Upper Salmon River at rkm 437</t>
+  </si>
+  <si>
+    <t>Upper Salmon River at rkm 460</t>
+  </si>
+  <si>
+    <t>522.303.437</t>
+  </si>
+  <si>
+    <t>522.303.460</t>
   </si>
 </sst>
 </file>
@@ -752,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -802,10 +808,10 @@
         <v>35</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -837,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -869,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -901,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -933,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1800,100 +1806,94 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="1">
+        <v>45.176475000000003</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-113.885278</v>
+      </c>
+      <c r="G33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="1">
+        <v>45.115074</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-113.774021</v>
+      </c>
+      <c r="G34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="1">
-        <v>45.176475000000003</v>
+        <v>45.113169999999997</v>
       </c>
       <c r="F35" s="1">
-        <v>-113.885278</v>
+        <v>-113.7556</v>
       </c>
       <c r="G35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="1" t="b">
         <v>1</v>
@@ -1902,24 +1902,24 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E36" s="1">
-        <v>45.115074</v>
+        <v>45.112769999999998</v>
       </c>
       <c r="F36" s="1">
-        <v>-113.774021</v>
+        <v>-113.74987</v>
       </c>
       <c r="G36" s="1" t="b">
         <v>0</v>
@@ -1931,315 +1931,315 @@
         <v>1</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="1">
+        <v>45.112189000000001</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-113.746897</v>
+      </c>
+      <c r="G37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="1">
-        <v>45.113169999999997</v>
-      </c>
-      <c r="F37" s="1">
-        <v>-113.7556</v>
-      </c>
-      <c r="G37" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E38" s="1">
-        <v>45.112769999999998</v>
+        <v>45.111257000000002</v>
       </c>
       <c r="F38" s="1">
-        <v>-113.74987</v>
+        <v>-113.74641800000001</v>
       </c>
       <c r="G38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="1">
+        <v>45.109456999999999</v>
+      </c>
+      <c r="F39" s="1">
+        <v>-113.742696</v>
+      </c>
+      <c r="G39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E39" s="1">
-        <v>45.112189000000001</v>
-      </c>
-      <c r="F39" s="1">
-        <v>-113.746897</v>
-      </c>
-      <c r="G39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="C40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="1">
+        <v>45.100087000000002</v>
+      </c>
+      <c r="F40" s="1">
+        <v>-113.72604200000001</v>
+      </c>
+      <c r="G40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="1">
-        <v>45.111257000000002</v>
-      </c>
-      <c r="F40" s="1">
-        <v>-113.74641800000001</v>
-      </c>
-      <c r="G40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="C41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="1">
+        <v>45.097937999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-113.72049699999999</v>
+      </c>
+      <c r="G41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E41" s="1">
-        <v>45.109456999999999</v>
-      </c>
-      <c r="F41" s="1">
-        <v>-113.742696</v>
-      </c>
-      <c r="G41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="1">
+        <v>45.026792</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-113.654847</v>
+      </c>
+      <c r="G42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="1">
-        <v>45.100087000000002</v>
-      </c>
-      <c r="F42" s="1">
-        <v>-113.72604200000001</v>
-      </c>
-      <c r="G42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="1">
+        <v>44.956738999999999</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-113.639543</v>
+      </c>
+      <c r="G43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="1">
-        <v>45.097937999999999</v>
-      </c>
-      <c r="F43" s="1">
-        <v>-113.72049699999999</v>
-      </c>
-      <c r="G43" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="1">
+        <v>44.865960029999997</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-113.62472099999999</v>
+      </c>
+      <c r="G44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" s="1">
-        <v>45.026792</v>
-      </c>
-      <c r="F44" s="1">
-        <v>-113.654847</v>
-      </c>
-      <c r="G44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="D45" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E45" s="1">
-        <v>44.956738999999999</v>
+        <v>44.861654000000001</v>
       </c>
       <c r="F45" s="1">
-        <v>-113.639543</v>
+        <v>-113.63193699999999</v>
       </c>
       <c r="G45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E46" s="1">
-        <v>44.865960029999997</v>
+        <v>45.028530000000003</v>
       </c>
       <c r="F46" s="1">
-        <v>-113.62472099999999</v>
+        <v>-113.916319</v>
       </c>
       <c r="G46" s="1" t="b">
         <v>1</v>
@@ -2251,27 +2251,27 @@
         <v>1</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E47" s="1">
-        <v>44.861654000000001</v>
+        <v>44.889763000000002</v>
       </c>
       <c r="F47" s="1">
-        <v>-113.63193699999999</v>
+        <v>-113.964145</v>
       </c>
       <c r="G47" s="1" t="b">
         <v>1</v>
@@ -2283,11 +2283,8 @@
         <v>1</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D48" s="5"/>
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor edit to fixed site metadata
</commit_message>
<xml_diff>
--- a/data/prepped/site_metadata/rt_site_metadata.xlsx
+++ b/data/prepped/site_metadata/rt_site_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\site_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB667974-4979-400F-A58C-7DAB6D51299E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE49F4F-E814-43A0-9904-09B2F8EA0A68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
   <si>
     <t>site_name</t>
   </si>
@@ -309,9 +309,6 @@
     <t>ptagis_rkm</t>
   </si>
   <si>
-    <t>rt_rkm</t>
-  </si>
-  <si>
     <t>522.303.416.001</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>522.303.460</t>
+  </si>
+  <si>
+    <t>522.303.103</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -779,7 +779,7 @@
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -810,11 +810,8 @@
       <c r="J1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -843,10 +840,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -875,10 +872,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -907,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -939,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -974,7 +971,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -1006,7 +1003,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -1038,7 +1035,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -1070,7 +1067,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -1134,7 +1131,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
@@ -1198,7 +1195,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -1230,7 +1227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1262,7 +1259,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1803,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -1835,12 +1832,12 @@
         <v>1</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>77</v>
@@ -1867,12 +1864,12 @@
         <v>1</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>78</v>
@@ -1899,12 +1896,12 @@
         <v>1</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>79</v>
@@ -1931,12 +1928,12 @@
         <v>1</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>80</v>
@@ -1963,12 +1960,12 @@
         <v>1</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>81</v>
@@ -1995,12 +1992,12 @@
         <v>1</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>82</v>
@@ -2027,12 +2024,12 @@
         <v>1</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>83</v>
@@ -2059,12 +2056,12 @@
         <v>1</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>84</v>
@@ -2091,12 +2088,12 @@
         <v>0</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>85</v>
@@ -2123,12 +2120,12 @@
         <v>1</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>86</v>
@@ -2155,12 +2152,12 @@
         <v>0</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>87</v>
@@ -2187,12 +2184,12 @@
         <v>1</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>88</v>
@@ -2219,15 +2216,15 @@
         <v>1</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>89</v>
@@ -2251,15 +2248,15 @@
         <v>1</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>89</v>
@@ -2283,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added summarise_test_data() and roxygenized package
</commit_message>
<xml_diff>
--- a/data/prepped/site_metadata/rt_site_metadata.xlsx
+++ b/data/prepped/site_metadata/rt_site_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\site_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC411A0-7183-4DD5-9CA2-5B05EEB5806F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D95B2C8-65E4-4508-A34D-CD289D2ABC3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_metadata" sheetId="1" r:id="rId1"/>
@@ -962,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2742,7 +2742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06388B40-C212-4A88-BF5F-9E1D4C67C429}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added site_metadata data with documentation, plus fixed minor formatting issues in rt_site_metadata.xlsx
</commit_message>
<xml_diff>
--- a/data/prepped/site_metadata/rt_site_metadata.xlsx
+++ b/data/prepped/site_metadata/rt_site_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\telemetyr\data\prepped\site_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D95B2C8-65E4-4508-A34D-CD289D2ABC3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34478FC-AA15-43FA-AD97-69EA98861BB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_metadata" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="199">
   <si>
     <t>site_name</t>
   </si>
@@ -605,6 +605,30 @@
   </si>
   <si>
     <t>RV2</t>
+  </si>
+  <si>
+    <t>274.044</t>
+  </si>
+  <si>
+    <t>335.002</t>
+  </si>
+  <si>
+    <t>274.042</t>
+  </si>
+  <si>
+    <t>274.031</t>
+  </si>
+  <si>
+    <t>274.028</t>
+  </si>
+  <si>
+    <t>274.025</t>
+  </si>
+  <si>
+    <t>274.007</t>
+  </si>
+  <si>
+    <t>274.005</t>
   </si>
 </sst>
 </file>
@@ -962,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -1054,8 +1078,8 @@
       <c r="K2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="10">
-        <v>274.04399999999998</v>
+      <c r="L2" s="10" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1168,8 +1192,8 @@
       <c r="K5" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="10">
-        <v>335.00200000000001</v>
+      <c r="L5" s="10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1206,8 +1230,8 @@
       <c r="K6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="10">
-        <v>274.04199999999997</v>
+      <c r="L6" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1244,8 +1268,8 @@
       <c r="K7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="10">
-        <v>274.03100000000001</v>
+      <c r="L7" s="10" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1282,8 +1306,8 @@
       <c r="K8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="10">
-        <v>274.02800000000002</v>
+      <c r="L8" s="10" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1320,8 +1344,8 @@
       <c r="K9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="10">
-        <v>274.02499999999998</v>
+      <c r="L9" s="10" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1358,8 +1382,8 @@
       <c r="K10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="10">
-        <v>274.01799999999997</v>
+      <c r="L10" s="10" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1396,8 +1420,8 @@
       <c r="K11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="10">
-        <v>274.01299999999998</v>
+      <c r="L11" s="10" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1434,8 +1458,8 @@
       <c r="K12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="10">
-        <v>274.00700000000001</v>
+      <c r="L12" s="10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1472,8 +1496,8 @@
       <c r="K13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="10">
-        <v>274.005</v>
+      <c r="L13" s="10" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2733,7 +2757,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="L17:L46" numberStoredAsText="1"/>
+    <ignoredError sqref="L17:L46 L2 L5:L13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>